<commit_message>
docs: Se Modifican Pruebas
</commit_message>
<xml_diff>
--- a/4- Evaluación/02 - Pruebas/01 - Pruebas.xlsx
+++ b/4- Evaluación/02 - Pruebas/01 - Pruebas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1803170\Proyecto_Tecnologico\Kyukeisho_New\4-Trimestre\Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1803170 - G3\Proyecto_Formativo\Kyukeisho_New\4- Evaluación\02 - Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBCE958-E183-42E6-932F-8A55FA8EA3BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C524EAB-C3A1-43AF-833B-9997436DF9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FCA5D05B-92FB-4B08-B387-7A93747DDFCB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Valores De Prueba</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Recupera contraseña</t>
+  </si>
+  <si>
+    <t>Crud Usuario</t>
+  </si>
+  <si>
+    <t>Crud Productos</t>
   </si>
 </sst>
 </file>
@@ -201,6 +207,32 @@
     <tableColumn id="2" xr3:uid="{7441A3D0-07FB-4A73-82E0-AA47CB6D048C}" name="Accion"/>
     <tableColumn id="3" xr3:uid="{B23D614B-8AD4-49A6-9F7A-385523192A38}" name="Resultado Esperado"/>
     <tableColumn id="4" xr3:uid="{1838E560-C0DE-456A-AD9D-A703E38B983A}" name="Resultado Obtenido"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D63FC376-3A88-493F-A625-71FB922851CB}" name="Tabla24" displayName="Tabla24" ref="A18:D22" totalsRowShown="0">
+  <autoFilter ref="A18:D22" xr:uid="{F0EB107B-AC08-4C45-8FC8-C619D8DAD6AC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4EDF1BC0-72F1-4E9C-B141-C4FA4B58B094}" name="Valores De Prueba"/>
+    <tableColumn id="2" xr3:uid="{B5763E61-C87B-4606-9A72-CF8FA8B7A5CF}" name="Accion"/>
+    <tableColumn id="3" xr3:uid="{DE0DE079-3E53-4228-A300-4D947A4310D2}" name="Resultado Esperado"/>
+    <tableColumn id="4" xr3:uid="{2FDF88B1-D418-4F5F-81FA-2DE3FCA49563}" name="Resultado Obtenido"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC3F1F4D-1D96-46EF-8FB8-1D92EB47416F}" name="Tabla245" displayName="Tabla245" ref="A25:D29" totalsRowShown="0">
+  <autoFilter ref="A25:D29" xr:uid="{F3D6F8E3-04AE-452B-9EDD-B154423FBE5E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{60F36E69-6672-4748-B918-09B78E7AB8CD}" name="Valores De Prueba"/>
+    <tableColumn id="2" xr3:uid="{A9562D57-F51B-4B8F-A8C4-3EA75C5BCCC8}" name="Accion"/>
+    <tableColumn id="3" xr3:uid="{16904B80-EADB-435C-8664-69A7AE0A4B3B}" name="Resultado Esperado"/>
+    <tableColumn id="4" xr3:uid="{F75EF1B1-B7EF-48FC-8E1F-3A29AB160DD5}" name="Resultado Obtenido"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD29347-0256-4E68-89E9-6EB61A74A7DA}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,16 +732,64 @@
         <v>24</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: Se Actualiza Aplicativo
</commit_message>
<xml_diff>
--- a/4- Evaluación/02 - Pruebas/01 - Pruebas.xlsx
+++ b/4- Evaluación/02 - Pruebas/01 - Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APRENDIZ SENA\SENA CEET ADSI\Kyukeisho_New\4- Evaluación\02 - Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED73A52-C9C3-4075-963B-A0F84AE9FAAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE4A8B3-F2E3-4851-9FA6-A2E3CE6B0A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCA5D05B-92FB-4B08-B387-7A93747DDFCB}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Ingresa</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Correo sin .com</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Agregar Producto</t>
+  </si>
+  <si>
+    <t>Login(Caja Blanca)</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -675,7 +675,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -711,63 +711,63 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
         <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -789,43 +789,43 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -847,35 +847,35 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>